<commit_message>
finishing environmental data and maps
</commit_message>
<xml_diff>
--- a/environmental_data/results_csv/temp_summary_30_5.xlsx
+++ b/environmental_data/results_csv/temp_summary_30_5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://miamiedu-my.sharepoint.com/personal/and128_miami_edu/Documents/GitHub/Ch2_AcerCCC/environmental_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://miamiedu-my.sharepoint.com/personal/and128_miami_edu/Documents/GitHub/Ch2_AcerCCC/environmental_data/results_csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{661683C0-2E69-FD40-B0DE-AD5F671E9582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2D3A427-DAEA-6645-B90A-FF054C5B31D3}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{661683C0-2E69-FD40-B0DE-AD5F671E9582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CBA510A-1F7E-7946-B626-60B56C34CAE3}"/>
   <bookViews>
-    <workbookView xWindow="50080" yWindow="3820" windowWidth="28040" windowHeight="16140" xr2:uid="{74A0D6DB-6026-BC4D-AFE4-FF1C41940A1C}"/>
+    <workbookView xWindow="12580" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{74A0D6DB-6026-BC4D-AFE4-FF1C41940A1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,7 +471,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,22 +502,22 @@
         <v>5</v>
       </c>
       <c r="B2" s="5">
-        <v>20.049099999999999</v>
+        <v>20.197679999999998</v>
       </c>
       <c r="C2" s="5">
         <v>31.817299999999999</v>
       </c>
-      <c r="D2" s="4">
-        <v>5.98</v>
+      <c r="D2" s="5">
+        <v>5.9773759999999996</v>
       </c>
       <c r="E2" s="4">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F2" s="5">
-        <v>0.80762929999999999</v>
+        <v>0.68933949999999999</v>
       </c>
       <c r="G2" s="5">
-        <v>11.7682</v>
+        <v>11.619619999999999</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -530,14 +530,14 @@
       <c r="C3" s="5">
         <v>31.472000000000001</v>
       </c>
-      <c r="D3" s="4">
-        <v>3.62</v>
+      <c r="D3" s="5">
+        <v>3.6226669999999999</v>
       </c>
       <c r="E3" s="4">
         <v>41</v>
       </c>
       <c r="F3" s="5">
-        <v>0.79891789999999996</v>
+        <v>0.71483540000000001</v>
       </c>
       <c r="G3" s="5">
         <v>9.9030000000000005</v>

</xml_diff>